<commit_message>
Timer & General Reqs
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1474FE-CDE8-4D03-BCE3-5BB65AA024A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D31EB3C-BCB4-4C56-9D23-4B7504BD1B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
@@ -794,6 +794,63 @@
     <t>The module shall increment the MM:SS:mm timer in BCD on o_count every rising edge of i_rtcclk if i_reset_n='1' and i_latchcount='1'  unless o_count is due to roll over to "000000000000000000000000"</t>
   </si>
   <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>TOP_INIT_01</t>
+  </si>
+  <si>
+    <t>Clocking</t>
+  </si>
+  <si>
+    <t>TOP_CLK_01</t>
+  </si>
+  <si>
+    <t>Module shall receive 100MHz Xilinx Artix-7 clock to use as sclk.</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>TOP_IN_01</t>
+  </si>
+  <si>
+    <t>Module shall use FPGA hardware pushbutton trigger_n as input to Trigger Detection module.</t>
+  </si>
+  <si>
+    <t>Module Instantiation</t>
+  </si>
+  <si>
+    <t>TOP_INST_01</t>
+  </si>
+  <si>
+    <t>Module shall pass sclk and reset_n to Trigger Detection, 10ms Timer, BCD to 7-Seg and 7-Seg module instantiations.</t>
+  </si>
+  <si>
+    <t>TOP_INST_02</t>
+  </si>
+  <si>
+    <t>Module shall pass only reset_n to 20-bit Counter.</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>TOP_OUT_01</t>
+  </si>
+  <si>
+    <t>Module shall display out current state of stopwatch system.</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>TOP_RST_01</t>
+  </si>
+  <si>
+    <t>Module shall update reset_n asynchronously</t>
+  </si>
+  <si>
     <t>TIMER</t>
   </si>
   <si>
@@ -824,70 +881,13 @@
     <t>Module shall invert o_basetick output once count equals 1000000 / 2</t>
   </si>
   <si>
-    <t>Reset</t>
-  </si>
-  <si>
     <t>TIMER_RST_01</t>
   </si>
   <si>
     <t>Module shall set internal counter to value of 0 when system reset input is logic low.</t>
   </si>
   <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>TOP_INIT_01</t>
-  </si>
-  <si>
-    <t>Clocking</t>
-  </si>
-  <si>
-    <t>TOP_CLK_01</t>
-  </si>
-  <si>
-    <t>Module shall receive 100MHz Xilinx Artix-7 clock to use as sclk.</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>TOP_IN_01</t>
-  </si>
-  <si>
-    <t>Module shall use FPGA hardware pushbutton trigger_n as input to Trigger Detection module.</t>
-  </si>
-  <si>
-    <t>Module Instantiation</t>
-  </si>
-  <si>
-    <t>TOP_INST_01</t>
-  </si>
-  <si>
-    <t>Module shall pass sclk and reset_n to Trigger Detection, 10ms Timer, BCD to 7-Seg and 7-Seg module instantiations.</t>
-  </si>
-  <si>
-    <t>TOP_INST_02</t>
-  </si>
-  <si>
-    <t>Module shall pass only reset_n to 20-bit Counter.</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>TOP_OUT_01</t>
-  </si>
-  <si>
-    <t>Module shall display out current state of stopwatch system.</t>
-  </si>
-  <si>
-    <t>TOP_RST_01</t>
-  </si>
-  <si>
-    <t>Module shall update reset_n asynchronously</t>
-  </si>
-  <si>
-    <t>Module shall toggle reset_n logic low in order to trigger system reset then passed to sub-modules.</t>
+    <t>Module shall toggle reset_n logic low ('0') for short period to trigger system reset passed to sub-modules.</t>
   </si>
 </sst>
 </file>
@@ -1569,47 +1569,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -1619,8 +1578,138 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -1631,82 +1720,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -1717,22 +1735,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -1744,51 +1781,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -2021,51 +2021,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="60" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="61" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2075,8 +2051,32 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="63" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="55" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -2395,7 +2395,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,20 +2624,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B832A1-37E9-4B2E-807C-B34D7E444DA2}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="99" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="90.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="106" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="89" t="s">
@@ -2652,60 +2652,60 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
-        <v>252</v>
-      </c>
-      <c r="B2" s="91" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="92" t="s">
-        <v>253</v>
-      </c>
-      <c r="D2" s="93" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="108" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95" t="s">
-        <v>255</v>
-      </c>
-      <c r="D3" s="96" t="s">
-        <v>256</v>
+      <c r="B3" s="105"/>
+      <c r="C3" s="110" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="111" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="73"/>
-      <c r="B4" s="91" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" s="92" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="93" t="s">
-        <v>259</v>
+      <c r="B4" s="107" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" s="108" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="109" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="73"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="97" t="s">
-        <v>260</v>
-      </c>
-      <c r="D5" s="96" t="s">
-        <v>261</v>
+      <c r="B5" s="105"/>
+      <c r="C5" s="112" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
-      <c r="B6" s="88" t="s">
-        <v>262</v>
-      </c>
-      <c r="C6" s="98" t="s">
-        <v>263</v>
-      </c>
-      <c r="D6" s="99" t="s">
-        <v>264</v>
+      <c r="A6" s="105"/>
+      <c r="B6" s="106" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="113" t="s">
+        <v>281</v>
+      </c>
+      <c r="D6" s="114" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B94154-4E96-428E-BDF1-A1ABE2650270}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C60" activeCellId="3" sqref="C54 C56 C58 C60"/>
     </sheetView>
   </sheetViews>
@@ -4087,20 +4087,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="104.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="106.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="88" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="89" t="s">
@@ -4114,87 +4114,87 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="94" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="95"/>
+      <c r="B3" s="92" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="97" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="95"/>
+      <c r="B4" s="92" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="95"/>
+      <c r="B5" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="99" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="95"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="102" t="s">
+        <v>263</v>
+      </c>
+      <c r="D6" s="103" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="95"/>
+      <c r="B7" s="92" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="102" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="103" t="s">
+      <c r="C7" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="D2" s="104" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="105"/>
-      <c r="B3" s="102" t="s">
+      <c r="D7" s="104" t="s">
         <v>267</v>
       </c>
-      <c r="C3" s="106" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="105"/>
+      <c r="B8" s="92" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="C8" s="93" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="105"/>
-      <c r="B4" s="102" t="s">
+      <c r="D8" s="94" t="s">
         <v>270</v>
-      </c>
-      <c r="C4" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="104" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="105"/>
-      <c r="B5" s="108" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" s="109" t="s">
-        <v>274</v>
-      </c>
-      <c r="D5" s="110" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="112" t="s">
-        <v>276</v>
-      </c>
-      <c r="D6" s="113" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="105"/>
-      <c r="B7" s="102" t="s">
-        <v>278</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="D7" s="114" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="94"/>
-      <c r="B8" s="102" t="s">
-        <v>262</v>
-      </c>
-      <c r="C8" s="103" t="s">
-        <v>281</v>
-      </c>
-      <c r="D8" s="104" t="s">
-        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reqs changes to adhere to Eric checklist rev2
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D31EB3C-BCB4-4C56-9D23-4B7504BD1B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62CFC4EF-0881-462B-863F-FA2B3685CBB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="282">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -794,6 +794,33 @@
     <t>The module shall increment the MM:SS:mm timer in BCD on o_count every rising edge of i_rtcclk if i_reset_n='1' and i_latchcount='1'  unless o_count is due to roll over to "000000000000000000000000"</t>
   </si>
   <si>
+    <t>TIMER</t>
+  </si>
+  <si>
+    <t>TIMER_INIT_01</t>
+  </si>
+  <si>
+    <t>Module shall set o_basetick logic low when i_reset_n is logic low.</t>
+  </si>
+  <si>
+    <t>Counting</t>
+  </si>
+  <si>
+    <t>TIMER_CNT_01</t>
+  </si>
+  <si>
+    <t>TIMER_CNT_02</t>
+  </si>
+  <si>
+    <t>Module shall invert o_basetick output once count equals 1000000 / 2</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>TIMER_RST_01</t>
+  </si>
+  <si>
     <t>TOP</t>
   </si>
   <si>
@@ -830,9 +857,6 @@
     <t>TOP_INST_02</t>
   </si>
   <si>
-    <t>Module shall pass only reset_n to 20-bit Counter.</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -842,52 +866,22 @@
     <t>Module shall display out current state of stopwatch system.</t>
   </si>
   <si>
-    <t>Reset</t>
-  </si>
-  <si>
     <t>TOP_RST_01</t>
   </si>
   <si>
-    <t>Module shall update reset_n asynchronously</t>
-  </si>
-  <si>
-    <t>TIMER</t>
-  </si>
-  <si>
-    <t>TIMER_INIT_01</t>
-  </si>
-  <si>
-    <t>Module shall set count to value of 0 when i_reset_n is logic low.</t>
-  </si>
-  <si>
-    <t>TIMER_INIT_02</t>
-  </si>
-  <si>
-    <t>Module shall set o_basetick logic low when i_reset_n is logic low.</t>
-  </si>
-  <si>
-    <t>Counting</t>
-  </si>
-  <si>
-    <t>TIMER_CNT_01</t>
-  </si>
-  <si>
-    <t>Module shall increment count on every positive edge of 100MHz i_sclk input when i_timerenb is high.</t>
-  </si>
-  <si>
-    <t>TIMER_CNT_02</t>
-  </si>
-  <si>
-    <t>Module shall invert o_basetick output once count equals 1000000 / 2</t>
-  </si>
-  <si>
-    <t>TIMER_RST_01</t>
-  </si>
-  <si>
-    <t>Module shall set internal counter to value of 0 when system reset input is logic low.</t>
-  </si>
-  <si>
-    <t>Module shall toggle reset_n logic low ('0') for short period to trigger system reset passed to sub-modules.</t>
+    <t>Module shall increment count on every positive edge of 100MHz i_sclk when i_timerenb is high.</t>
+  </si>
+  <si>
+    <t>Module shall set internal counter to value of 0 when i_reset_n is logic low.</t>
+  </si>
+  <si>
+    <t>Module shall set reset_n logic low ('0') for short period to trigger system reset.</t>
+  </si>
+  <si>
+    <t>Module shall show only zeroes across all 7-seg displays when reset_n is set logic low ('0').</t>
+  </si>
+  <si>
+    <t>Module shall pass only reset_n to 24-bit Counter.</t>
   </si>
 </sst>
 </file>
@@ -955,7 +949,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="64">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1569,6 +1563,47 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -1578,13 +1613,30 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1594,21 +1646,57 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1679,112 +1767,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -1799,7 +1786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2021,27 +2008,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="59" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2051,32 +2047,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="55" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="61" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -2622,22 +2601,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B832A1-37E9-4B2E-807C-B34D7E444DA2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="90.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="88" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="89" t="s">
@@ -2650,69 +2629,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" s="107" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="108" t="s">
-        <v>272</v>
-      </c>
-      <c r="D2" s="109" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="111" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="112" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="73"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="110" t="s">
-        <v>274</v>
-      </c>
-      <c r="D3" s="111" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="103" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="92" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73"/>
-      <c r="B4" s="107" t="s">
-        <v>276</v>
-      </c>
-      <c r="C4" s="108" t="s">
-        <v>277</v>
-      </c>
-      <c r="D4" s="109" t="s">
+      <c r="B4" s="106"/>
+      <c r="C4" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" s="93" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="74"/>
+      <c r="B5" s="88" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" s="96" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="112" t="s">
-        <v>279</v>
-      </c>
-      <c r="D5" s="111" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="106" t="s">
-        <v>268</v>
-      </c>
-      <c r="C6" s="113" t="s">
-        <v>281</v>
-      </c>
-      <c r="D6" s="114" t="s">
-        <v>282</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4087,20 +4055,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="106.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="105.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="89" t="s">
@@ -4114,87 +4082,87 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
-        <v>252</v>
-      </c>
-      <c r="B2" s="92" t="s">
+      <c r="A2" s="110" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="93" t="s">
-        <v>253</v>
-      </c>
-      <c r="D2" s="94" t="s">
-        <v>283</v>
+      <c r="C2" s="99" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="95"/>
-      <c r="B3" s="92" t="s">
-        <v>254</v>
-      </c>
-      <c r="C3" s="96" t="s">
-        <v>255</v>
-      </c>
-      <c r="D3" s="97" t="s">
-        <v>256</v>
+      <c r="A3" s="73"/>
+      <c r="B3" s="98" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="101" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="102" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="95"/>
-      <c r="B4" s="92" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" s="93" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="94" t="s">
+      <c r="A4" s="73"/>
+      <c r="B4" s="98" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="99" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="100" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="73"/>
+      <c r="B5" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="104" t="s">
+        <v>270</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="73"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="107" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="108" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="73"/>
+      <c r="B7" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" s="109" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="74"/>
+      <c r="B8" s="98" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="95"/>
-      <c r="B5" s="98" t="s">
-        <v>260</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" s="100" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="95"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="102" t="s">
-        <v>263</v>
-      </c>
-      <c r="D6" s="103" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="95"/>
-      <c r="B7" s="92" t="s">
-        <v>265</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="D7" s="104" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="105"/>
-      <c r="B8" s="92" t="s">
-        <v>268</v>
-      </c>
-      <c r="C8" s="93" t="s">
-        <v>269</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>270</v>
+      <c r="C8" s="99" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" s="100" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4207,6 +4175,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11c68bd7e868490b50c80001f2cf6c52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" xmlns:ns3="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7feae6b8f12256f9c4998c90aa2e28a" ns2:_="" ns3:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -4385,7 +4359,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4394,13 +4368,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4419,19 +4396,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reqs changes for revision 3
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62CFC4EF-0881-462B-863F-FA2B3685CBB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9297BB-AF36-4574-95B6-F4437BFCA6A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="280">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -812,9 +812,6 @@
     <t>TIMER_CNT_02</t>
   </si>
   <si>
-    <t>Module shall invert o_basetick output once count equals 1000000 / 2</t>
-  </si>
-  <si>
     <t>Reset</t>
   </si>
   <si>
@@ -824,9 +821,6 @@
     <t>TOP</t>
   </si>
   <si>
-    <t>TOP_INIT_01</t>
-  </si>
-  <si>
     <t>Clocking</t>
   </si>
   <si>
@@ -869,19 +863,19 @@
     <t>TOP_RST_01</t>
   </si>
   <si>
-    <t>Module shall increment count on every positive edge of 100MHz i_sclk when i_timerenb is high.</t>
-  </si>
-  <si>
-    <t>Module shall set internal counter to value of 0 when i_reset_n is logic low.</t>
-  </si>
-  <si>
-    <t>Module shall set reset_n logic low ('0') for short period to trigger system reset.</t>
-  </si>
-  <si>
     <t>Module shall show only zeroes across all 7-seg displays when reset_n is set logic low ('0').</t>
   </si>
   <si>
     <t>Module shall pass only reset_n to 24-bit Counter.</t>
+  </si>
+  <si>
+    <t>Module shall increment count on every positive edge of 100MHz i_sclk when i_timerenb is logic high.</t>
+  </si>
+  <si>
+    <t>Module shall set count to value of 0 when i_reset_n is logic low.</t>
+  </si>
+  <si>
+    <t>Module shall invert o_basetick output once count equals 500000.</t>
   </si>
 </sst>
 </file>
@@ -1689,21 +1683,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -1779,6 +1758,19 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1786,7 +1778,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1951,54 +1943,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2023,39 +1967,84 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="58" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="59" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="60" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="61" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -2400,10 +2389,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2414,8 +2403,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
       <c r="C3" s="54" t="s">
         <v>5</v>
       </c>
@@ -2424,8 +2413,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
       <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
@@ -2434,8 +2423,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
       <c r="C5" s="54" t="s">
         <v>25</v>
       </c>
@@ -2444,8 +2433,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="73"/>
-      <c r="B6" s="74"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="14" t="s">
         <v>26</v>
       </c>
@@ -2454,8 +2443,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73" t="s">
+      <c r="A7" s="94"/>
+      <c r="B7" s="94" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="56" t="s">
@@ -2466,8 +2455,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
@@ -2476,8 +2465,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="58" t="s">
         <v>38</v>
       </c>
@@ -2486,8 +2475,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="73"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
@@ -2496,8 +2485,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73"/>
-      <c r="B11" s="76"/>
+      <c r="A11" s="94"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="60" t="s">
         <v>19</v>
       </c>
@@ -2506,8 +2495,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="72" t="s">
+      <c r="A12" s="94"/>
+      <c r="B12" s="93" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2518,8 +2507,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="73"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="56" t="s">
         <v>22</v>
       </c>
@@ -2528,8 +2517,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="8" t="s">
         <v>23</v>
       </c>
@@ -2538,8 +2527,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="74"/>
-      <c r="B15" s="74"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="95"/>
       <c r="C15" s="62" t="s">
         <v>27</v>
       </c>
@@ -2604,7 +2593,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,64 +2605,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="74" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="96" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="91" t="s">
         <v>253</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="92" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
-      <c r="B3" s="103" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="98" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="75" t="s">
         <v>256</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="76" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="73"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="94" t="s">
+      <c r="A4" s="94"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="77" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="95"/>
+      <c r="B5" s="72" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74"/>
-      <c r="B5" s="88" t="s">
+      <c r="C5" s="79" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="95" t="s">
-        <v>260</v>
-      </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="80" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2718,10 +2707,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="100" t="s">
         <v>223</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="100" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="66" t="s">
@@ -2732,8 +2721,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
-      <c r="B3" s="78"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
       <c r="C3" s="68" t="s">
         <v>226</v>
       </c>
@@ -2742,8 +2731,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
-      <c r="B4" s="78"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="68" t="s">
         <v>228</v>
       </c>
@@ -2752,8 +2741,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="70" t="s">
         <v>230</v>
       </c>
@@ -2762,8 +2751,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="78"/>
-      <c r="B6" s="77" t="s">
+      <c r="A6" s="101"/>
+      <c r="B6" s="100" t="s">
         <v>232</v>
       </c>
       <c r="C6" s="66" t="s">
@@ -2774,8 +2763,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
-      <c r="B7" s="78"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="68" t="s">
         <v>235</v>
       </c>
@@ -2784,8 +2773,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="68" t="s">
         <v>237</v>
       </c>
@@ -2794,8 +2783,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="68" t="s">
         <v>239</v>
       </c>
@@ -2804,8 +2793,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="68" t="s">
         <v>241</v>
       </c>
@@ -2814,8 +2803,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
-      <c r="B11" s="79"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="70" t="s">
         <v>243</v>
       </c>
@@ -2824,8 +2813,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="77" t="s">
+      <c r="A12" s="101"/>
+      <c r="B12" s="100" t="s">
         <v>245</v>
       </c>
       <c r="C12" s="66" t="s">
@@ -2836,8 +2825,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="78"/>
-      <c r="B13" s="78"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="101"/>
       <c r="C13" s="68" t="s">
         <v>248</v>
       </c>
@@ -2846,8 +2835,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
-      <c r="B14" s="79"/>
+      <c r="A14" s="102"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="70" t="s">
         <v>250</v>
       </c>
@@ -2899,10 +2888,10 @@
       <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="103" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="29" t="s">
@@ -2913,8 +2902,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
-      <c r="B3" s="81"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="104"/>
       <c r="C3" s="36" t="s">
         <v>10</v>
       </c>
@@ -2923,8 +2912,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
-      <c r="B4" s="81"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
@@ -2933,8 +2922,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
-      <c r="B5" s="81"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="36" t="s">
         <v>12</v>
       </c>
@@ -2943,8 +2932,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="78"/>
-      <c r="B6" s="81"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="30" t="s">
         <v>13</v>
       </c>
@@ -2953,8 +2942,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
-      <c r="B7" s="82" t="s">
+      <c r="A7" s="101"/>
+      <c r="B7" s="105" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -2965,8 +2954,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="30" t="s">
         <v>46</v>
       </c>
@@ -2975,8 +2964,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
@@ -2985,8 +2974,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="78"/>
-      <c r="B10" s="83"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="30" t="s">
         <v>50</v>
       </c>
@@ -2995,8 +2984,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="78"/>
-      <c r="B11" s="83"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
@@ -3005,8 +2994,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="83"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="30" t="s">
         <v>54</v>
       </c>
@@ -3015,8 +3004,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="78"/>
-      <c r="B13" s="83"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="2" t="s">
         <v>56</v>
       </c>
@@ -3025,8 +3014,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
-      <c r="B14" s="83"/>
+      <c r="A14" s="101"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="30" t="s">
         <v>58</v>
       </c>
@@ -3035,8 +3024,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="78"/>
-      <c r="B15" s="84"/>
+      <c r="A15" s="101"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="3" t="s">
         <v>60</v>
       </c>
@@ -3045,8 +3034,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="82" t="s">
+      <c r="A16" s="101"/>
+      <c r="B16" s="105" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="29" t="s">
@@ -3057,8 +3046,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="106"/>
       <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
@@ -3067,8 +3056,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="106"/>
       <c r="C18" s="30" t="s">
         <v>66</v>
       </c>
@@ -3077,8 +3066,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="106"/>
       <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
@@ -3087,8 +3076,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="78"/>
-      <c r="B20" s="83"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="106"/>
       <c r="C20" s="30" t="s">
         <v>70</v>
       </c>
@@ -3097,8 +3086,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="78"/>
-      <c r="B21" s="83"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="106"/>
       <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
@@ -3107,8 +3096,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="78"/>
-      <c r="B22" s="83"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="30" t="s">
         <v>74</v>
       </c>
@@ -3117,8 +3106,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="78"/>
-      <c r="B23" s="83"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="106"/>
       <c r="C23" s="2" t="s">
         <v>76</v>
       </c>
@@ -3127,8 +3116,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="78"/>
-      <c r="B24" s="84"/>
+      <c r="A24" s="101"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="32" t="s">
         <v>78</v>
       </c>
@@ -3137,8 +3126,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
-      <c r="B25" s="82" t="s">
+      <c r="A25" s="101"/>
+      <c r="B25" s="105" t="s">
         <v>80</v>
       </c>
       <c r="C25" s="25" t="s">
@@ -3149,8 +3138,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="101"/>
+      <c r="B26" s="106"/>
       <c r="C26" s="30" t="s">
         <v>82</v>
       </c>
@@ -3159,8 +3148,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="78"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="106"/>
       <c r="C27" s="2" t="s">
         <v>84</v>
       </c>
@@ -3169,8 +3158,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="101"/>
+      <c r="B28" s="106"/>
       <c r="C28" s="30" t="s">
         <v>86</v>
       </c>
@@ -3179,8 +3168,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="78"/>
-      <c r="B29" s="83"/>
+      <c r="A29" s="101"/>
+      <c r="B29" s="106"/>
       <c r="C29" s="2" t="s">
         <v>88</v>
       </c>
@@ -3189,8 +3178,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="78"/>
-      <c r="B30" s="83"/>
+      <c r="A30" s="101"/>
+      <c r="B30" s="106"/>
       <c r="C30" s="30" t="s">
         <v>90</v>
       </c>
@@ -3199,8 +3188,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="78"/>
-      <c r="B31" s="83"/>
+      <c r="A31" s="101"/>
+      <c r="B31" s="106"/>
       <c r="C31" s="2" t="s">
         <v>92</v>
       </c>
@@ -3209,8 +3198,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="78"/>
-      <c r="B32" s="83"/>
+      <c r="A32" s="101"/>
+      <c r="B32" s="106"/>
       <c r="C32" s="30" t="s">
         <v>94</v>
       </c>
@@ -3219,8 +3208,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="78"/>
-      <c r="B33" s="84"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="107"/>
       <c r="C33" s="27" t="s">
         <v>96</v>
       </c>
@@ -3229,8 +3218,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="78"/>
-      <c r="B34" s="82" t="s">
+      <c r="A34" s="101"/>
+      <c r="B34" s="105" t="s">
         <v>98</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -3241,8 +3230,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="78"/>
-      <c r="B35" s="83"/>
+      <c r="A35" s="101"/>
+      <c r="B35" s="106"/>
       <c r="C35" s="2" t="s">
         <v>100</v>
       </c>
@@ -3251,8 +3240,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="78"/>
-      <c r="B36" s="83"/>
+      <c r="A36" s="101"/>
+      <c r="B36" s="106"/>
       <c r="C36" s="30" t="s">
         <v>102</v>
       </c>
@@ -3261,8 +3250,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="78"/>
-      <c r="B37" s="83"/>
+      <c r="A37" s="101"/>
+      <c r="B37" s="106"/>
       <c r="C37" s="2" t="s">
         <v>104</v>
       </c>
@@ -3271,8 +3260,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="78"/>
-      <c r="B38" s="83"/>
+      <c r="A38" s="101"/>
+      <c r="B38" s="106"/>
       <c r="C38" s="30" t="s">
         <v>106</v>
       </c>
@@ -3281,8 +3270,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="78"/>
-      <c r="B39" s="83"/>
+      <c r="A39" s="101"/>
+      <c r="B39" s="106"/>
       <c r="C39" s="2" t="s">
         <v>108</v>
       </c>
@@ -3291,8 +3280,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="78"/>
-      <c r="B40" s="83"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="106"/>
       <c r="C40" s="30" t="s">
         <v>110</v>
       </c>
@@ -3301,8 +3290,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="78"/>
-      <c r="B41" s="83"/>
+      <c r="A41" s="101"/>
+      <c r="B41" s="106"/>
       <c r="C41" s="2" t="s">
         <v>112</v>
       </c>
@@ -3311,8 +3300,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="78"/>
-      <c r="B42" s="84"/>
+      <c r="A42" s="101"/>
+      <c r="B42" s="107"/>
       <c r="C42" s="32" t="s">
         <v>114</v>
       </c>
@@ -3321,8 +3310,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="78"/>
-      <c r="B43" s="82" t="s">
+      <c r="A43" s="101"/>
+      <c r="B43" s="105" t="s">
         <v>116</v>
       </c>
       <c r="C43" s="25" t="s">
@@ -3333,8 +3322,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="78"/>
-      <c r="B44" s="83"/>
+      <c r="A44" s="101"/>
+      <c r="B44" s="106"/>
       <c r="C44" s="30" t="s">
         <v>118</v>
       </c>
@@ -3343,8 +3332,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="78"/>
-      <c r="B45" s="83"/>
+      <c r="A45" s="101"/>
+      <c r="B45" s="106"/>
       <c r="C45" s="2" t="s">
         <v>120</v>
       </c>
@@ -3353,8 +3342,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="78"/>
-      <c r="B46" s="83"/>
+      <c r="A46" s="101"/>
+      <c r="B46" s="106"/>
       <c r="C46" s="30" t="s">
         <v>122</v>
       </c>
@@ -3363,8 +3352,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="78"/>
-      <c r="B47" s="83"/>
+      <c r="A47" s="101"/>
+      <c r="B47" s="106"/>
       <c r="C47" s="2" t="s">
         <v>124</v>
       </c>
@@ -3373,8 +3362,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="78"/>
-      <c r="B48" s="83"/>
+      <c r="A48" s="101"/>
+      <c r="B48" s="106"/>
       <c r="C48" s="30" t="s">
         <v>126</v>
       </c>
@@ -3383,8 +3372,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="78"/>
-      <c r="B49" s="83"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="106"/>
       <c r="C49" s="2" t="s">
         <v>128</v>
       </c>
@@ -3393,8 +3382,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="78"/>
-      <c r="B50" s="83"/>
+      <c r="A50" s="101"/>
+      <c r="B50" s="106"/>
       <c r="C50" s="30" t="s">
         <v>130</v>
       </c>
@@ -3403,8 +3392,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="78"/>
-      <c r="B51" s="84"/>
+      <c r="A51" s="101"/>
+      <c r="B51" s="107"/>
       <c r="C51" s="3" t="s">
         <v>132</v>
       </c>
@@ -3413,8 +3402,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="78"/>
-      <c r="B52" s="82" t="s">
+      <c r="A52" s="101"/>
+      <c r="B52" s="105" t="s">
         <v>134</v>
       </c>
       <c r="C52" s="29" t="s">
@@ -3425,8 +3414,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="78"/>
-      <c r="B53" s="83"/>
+      <c r="A53" s="101"/>
+      <c r="B53" s="106"/>
       <c r="C53" s="2" t="s">
         <v>142</v>
       </c>
@@ -3435,8 +3424,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="78"/>
-      <c r="B54" s="83"/>
+      <c r="A54" s="101"/>
+      <c r="B54" s="106"/>
       <c r="C54" s="30" t="s">
         <v>143</v>
       </c>
@@ -3445,8 +3434,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="78"/>
-      <c r="B55" s="83"/>
+      <c r="A55" s="101"/>
+      <c r="B55" s="106"/>
       <c r="C55" s="2" t="s">
         <v>144</v>
       </c>
@@ -3455,8 +3444,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="78"/>
-      <c r="B56" s="83"/>
+      <c r="A56" s="101"/>
+      <c r="B56" s="106"/>
       <c r="C56" s="30" t="s">
         <v>145</v>
       </c>
@@ -3465,8 +3454,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="78"/>
-      <c r="B57" s="83"/>
+      <c r="A57" s="101"/>
+      <c r="B57" s="106"/>
       <c r="C57" s="2" t="s">
         <v>146</v>
       </c>
@@ -3475,8 +3464,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="78"/>
-      <c r="B58" s="83"/>
+      <c r="A58" s="101"/>
+      <c r="B58" s="106"/>
       <c r="C58" s="30" t="s">
         <v>147</v>
       </c>
@@ -3485,8 +3474,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="78"/>
-      <c r="B59" s="83"/>
+      <c r="A59" s="101"/>
+      <c r="B59" s="106"/>
       <c r="C59" s="2" t="s">
         <v>148</v>
       </c>
@@ -3495,8 +3484,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="79"/>
-      <c r="B60" s="84"/>
+      <c r="A60" s="102"/>
+      <c r="B60" s="107"/>
       <c r="C60" s="32" t="s">
         <v>149</v>
       </c>
@@ -3551,10 +3540,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="100" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="110" t="s">
         <v>159</v>
       </c>
       <c r="C2" s="29" t="s">
@@ -3565,8 +3554,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
-      <c r="B3" s="85"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="36" t="s">
         <v>163</v>
       </c>
@@ -3575,8 +3564,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
-      <c r="B4" s="85"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="38" t="s">
         <v>186</v>
       </c>
@@ -3585,8 +3574,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78"/>
-      <c r="B5" s="86"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="40" t="s">
         <v>187</v>
       </c>
@@ -3595,8 +3584,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="78"/>
-      <c r="B6" s="85" t="s">
+      <c r="A6" s="101"/>
+      <c r="B6" s="108" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="38" t="s">
@@ -3607,8 +3596,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="78"/>
-      <c r="B7" s="86"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="43" t="s">
         <v>165</v>
       </c>
@@ -3617,8 +3606,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
-      <c r="B8" s="87" t="s">
+      <c r="A8" s="101"/>
+      <c r="B8" s="110" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="29" t="s">
@@ -3629,8 +3618,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="108"/>
       <c r="C9" s="42" t="s">
         <v>171</v>
       </c>
@@ -3639,8 +3628,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="78"/>
-      <c r="B10" s="85"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="108"/>
       <c r="C10" s="38" t="s">
         <v>172</v>
       </c>
@@ -3649,8 +3638,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="78"/>
-      <c r="B11" s="85"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="108"/>
       <c r="C11" s="42" t="s">
         <v>173</v>
       </c>
@@ -3659,8 +3648,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="85"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="108"/>
       <c r="C12" s="38" t="s">
         <v>177</v>
       </c>
@@ -3669,8 +3658,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="78"/>
-      <c r="B13" s="85"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="108"/>
       <c r="C13" s="42" t="s">
         <v>178</v>
       </c>
@@ -3679,8 +3668,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
-      <c r="B14" s="85"/>
+      <c r="A14" s="101"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="38" t="s">
         <v>179</v>
       </c>
@@ -3689,8 +3678,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="78"/>
-      <c r="B15" s="85"/>
+      <c r="A15" s="101"/>
+      <c r="B15" s="108"/>
       <c r="C15" s="45" t="s">
         <v>180</v>
       </c>
@@ -3699,8 +3688,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="82" t="s">
+      <c r="A16" s="101"/>
+      <c r="B16" s="105" t="s">
         <v>218</v>
       </c>
       <c r="C16" s="29" t="s">
@@ -3711,8 +3700,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="106"/>
       <c r="C17" s="2" t="s">
         <v>189</v>
       </c>
@@ -3721,8 +3710,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="101"/>
+      <c r="B18" s="106"/>
       <c r="C18" s="38" t="s">
         <v>191</v>
       </c>
@@ -3731,8 +3720,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="101"/>
+      <c r="B19" s="106"/>
       <c r="C19" s="2" t="s">
         <v>192</v>
       </c>
@@ -3741,8 +3730,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="78"/>
-      <c r="B20" s="83"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="106"/>
       <c r="C20" s="38" t="s">
         <v>193</v>
       </c>
@@ -3751,8 +3740,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="78"/>
-      <c r="B21" s="83"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="106"/>
       <c r="C21" s="2" t="s">
         <v>194</v>
       </c>
@@ -3761,8 +3750,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="78"/>
-      <c r="B22" s="83"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="38" t="s">
         <v>200</v>
       </c>
@@ -3771,8 +3760,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="78"/>
-      <c r="B23" s="83"/>
+      <c r="A23" s="101"/>
+      <c r="B23" s="106"/>
       <c r="C23" s="2" t="s">
         <v>201</v>
       </c>
@@ -3781,8 +3770,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="78"/>
-      <c r="B24" s="83"/>
+      <c r="A24" s="101"/>
+      <c r="B24" s="106"/>
       <c r="C24" s="38" t="s">
         <v>210</v>
       </c>
@@ -3791,8 +3780,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
-      <c r="B25" s="83"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="106"/>
       <c r="C25" s="2" t="s">
         <v>211</v>
       </c>
@@ -3801,8 +3790,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="101"/>
+      <c r="B26" s="106"/>
       <c r="C26" s="38" t="s">
         <v>212</v>
       </c>
@@ -3811,8 +3800,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="78"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="106"/>
       <c r="C27" s="2" t="s">
         <v>213</v>
       </c>
@@ -3821,8 +3810,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="101"/>
+      <c r="B28" s="106"/>
       <c r="C28" s="38" t="s">
         <v>214</v>
       </c>
@@ -3831,8 +3820,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
-      <c r="B29" s="84"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="107"/>
       <c r="C29" s="3" t="s">
         <v>215</v>
       </c>
@@ -4053,10 +4042,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4068,116 +4057,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="74" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="96" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="81" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="98" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="84" t="s">
         <v>262</v>
       </c>
-      <c r="D2" s="100" t="s">
-        <v>279</v>
+      <c r="D2" s="85" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="73"/>
-      <c r="B3" s="98" t="s">
-        <v>263</v>
-      </c>
-      <c r="C3" s="101" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="C3" s="82" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="73"/>
+      <c r="D3" s="83" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="94"/>
       <c r="B4" s="98" t="s">
-        <v>266</v>
-      </c>
-      <c r="C4" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="C4" s="86" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
-      <c r="B5" s="103" t="s">
+      <c r="D4" s="87" t="s">
         <v>269</v>
       </c>
-      <c r="C5" s="104" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="94"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="88" t="s">
         <v>270</v>
       </c>
-      <c r="D5" s="105" t="s">
+      <c r="D5" s="89" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="94"/>
+      <c r="B6" s="81" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="73"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="D6" s="108" t="s">
-        <v>281</v>
+      <c r="D6" s="90" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73"/>
-      <c r="B7" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="A7" s="95"/>
+      <c r="B7" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="D7" s="109" t="s">
+      <c r="D7" s="83" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74"/>
-      <c r="B8" s="98" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="99" t="s">
-        <v>276</v>
-      </c>
-      <c r="D8" s="100" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A2:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4360,19 +4340,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4397,9 +4373,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Design reviews and updated Requirements and Testcases
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9297BB-AF36-4574-95B6-F4437BFCA6A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8AE68FB-1485-4C99-B3A7-F15485BD3904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="General" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1988,6 +1989,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2041,9 +2045,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2366,15 +2367,15 @@
       <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="124.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="124.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="51" t="s">
         <v>2</v>
       </c>
@@ -2388,11 +2389,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="97" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2402,9 +2403,9 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="94"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="95"/>
+      <c r="B3" s="95"/>
       <c r="C3" s="54" t="s">
         <v>5</v>
       </c>
@@ -2412,9 +2413,9 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="94"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="95"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
@@ -2422,9 +2423,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
-      <c r="B5" s="94"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="95"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="54" t="s">
         <v>25</v>
       </c>
@@ -2432,9 +2433,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="95"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="14" t="s">
         <v>26</v>
       </c>
@@ -2442,9 +2443,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="94"/>
-      <c r="B7" s="94" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="95"/>
+      <c r="B7" s="95" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="56" t="s">
@@ -2454,9 +2455,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="95"/>
+      <c r="B8" s="95"/>
       <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
@@ -2464,9 +2465,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
-      <c r="B9" s="94"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="95"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="58" t="s">
         <v>38</v>
       </c>
@@ -2474,9 +2475,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
-      <c r="B10" s="94"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="95"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
@@ -2484,9 +2485,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="94"/>
-      <c r="B11" s="97"/>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="95"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="60" t="s">
         <v>19</v>
       </c>
@@ -2494,9 +2495,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
-      <c r="B12" s="93" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="95"/>
+      <c r="B12" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2506,9 +2507,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="95"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="56" t="s">
         <v>22</v>
       </c>
@@ -2516,9 +2517,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
-      <c r="B14" s="94"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="95"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="8" t="s">
         <v>23</v>
       </c>
@@ -2526,9 +2527,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="95"/>
-      <c r="B15" s="95"/>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="96"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="62" t="s">
         <v>27</v>
       </c>
@@ -2536,44 +2537,44 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C23"/>
       <c r="D23"/>
     </row>
@@ -2592,19 +2593,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B832A1-37E9-4B2E-807C-B34D7E444DA2}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" customWidth="1"/>
+    <col min="4" max="4" width="90.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="72" t="s">
         <v>2</v>
       </c>
@@ -2618,8 +2619,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="97" t="s">
         <v>252</v>
       </c>
       <c r="B2" s="81" t="s">
@@ -2632,9 +2633,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="98" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="95"/>
+      <c r="B3" s="99" t="s">
         <v>255</v>
       </c>
       <c r="C3" s="75" t="s">
@@ -2644,9 +2645,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="94"/>
-      <c r="B4" s="99"/>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="95"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="78" t="s">
         <v>257</v>
       </c>
@@ -2654,8 +2655,8 @@
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95"/>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="96"/>
       <c r="B5" s="72" t="s">
         <v>258</v>
       </c>
@@ -2683,16 +2684,16 @@
       <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="181.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="181.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="64" t="s">
         <v>14</v>
       </c>
@@ -2706,11 +2707,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="101" t="s">
         <v>223</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="101" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="66" t="s">
@@ -2720,9 +2721,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
-      <c r="B3" s="101"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="102"/>
+      <c r="B3" s="102"/>
       <c r="C3" s="68" t="s">
         <v>226</v>
       </c>
@@ -2730,9 +2731,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="101"/>
-      <c r="B4" s="101"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="102"/>
+      <c r="B4" s="102"/>
       <c r="C4" s="68" t="s">
         <v>228</v>
       </c>
@@ -2740,9 +2741,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="101"/>
-      <c r="B5" s="102"/>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="102"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="70" t="s">
         <v>230</v>
       </c>
@@ -2750,9 +2751,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="101"/>
-      <c r="B6" s="100" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="102"/>
+      <c r="B6" s="101" t="s">
         <v>232</v>
       </c>
       <c r="C6" s="66" t="s">
@@ -2762,9 +2763,9 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="101"/>
-      <c r="B7" s="101"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="102"/>
+      <c r="B7" s="102"/>
       <c r="C7" s="68" t="s">
         <v>235</v>
       </c>
@@ -2772,9 +2773,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="101"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="68" t="s">
         <v>237</v>
       </c>
@@ -2782,9 +2783,9 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="101"/>
-      <c r="B9" s="101"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="68" t="s">
         <v>239</v>
       </c>
@@ -2792,9 +2793,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="101"/>
-      <c r="B10" s="101"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="102"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="68" t="s">
         <v>241</v>
       </c>
@@ -2802,9 +2803,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101"/>
-      <c r="B11" s="102"/>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="102"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="70" t="s">
         <v>243</v>
       </c>
@@ -2812,9 +2813,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="101"/>
-      <c r="B12" s="100" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="102"/>
+      <c r="B12" s="101" t="s">
         <v>245</v>
       </c>
       <c r="C12" s="66" t="s">
@@ -2824,9 +2825,9 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="101"/>
-      <c r="B13" s="101"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="102"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="68" t="s">
         <v>248</v>
       </c>
@@ -2834,9 +2835,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="102"/>
-      <c r="B14" s="102"/>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="103"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="70" t="s">
         <v>250</v>
       </c>
@@ -2863,16 +2864,16 @@
       <selection activeCell="C60" activeCellId="3" sqref="C54 C56 C58 C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="146.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="146.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
@@ -2887,11 +2888,11 @@
       </c>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="104" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="29" t="s">
@@ -2901,9 +2902,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
-      <c r="B3" s="104"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="102"/>
+      <c r="B3" s="105"/>
       <c r="C3" s="36" t="s">
         <v>10</v>
       </c>
@@ -2911,9 +2912,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="101"/>
-      <c r="B4" s="104"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="102"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
@@ -2921,9 +2922,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="101"/>
-      <c r="B5" s="104"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="102"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="36" t="s">
         <v>12</v>
       </c>
@@ -2931,9 +2932,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="101"/>
-      <c r="B6" s="104"/>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="102"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="30" t="s">
         <v>13</v>
       </c>
@@ -2941,9 +2942,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="101"/>
-      <c r="B7" s="105" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="102"/>
+      <c r="B7" s="106" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -2953,9 +2954,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="106"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="102"/>
+      <c r="B8" s="107"/>
       <c r="C8" s="30" t="s">
         <v>46</v>
       </c>
@@ -2963,9 +2964,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="101"/>
-      <c r="B9" s="106"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="102"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
@@ -2973,9 +2974,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="101"/>
-      <c r="B10" s="106"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="102"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="30" t="s">
         <v>50</v>
       </c>
@@ -2983,9 +2984,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="101"/>
-      <c r="B11" s="106"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="102"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
@@ -2993,9 +2994,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="101"/>
-      <c r="B12" s="106"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="102"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="30" t="s">
         <v>54</v>
       </c>
@@ -3003,9 +3004,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="101"/>
-      <c r="B13" s="106"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="102"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="2" t="s">
         <v>56</v>
       </c>
@@ -3013,9 +3014,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="101"/>
-      <c r="B14" s="106"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="102"/>
+      <c r="B14" s="107"/>
       <c r="C14" s="30" t="s">
         <v>58</v>
       </c>
@@ -3023,9 +3024,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="101"/>
-      <c r="B15" s="107"/>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="102"/>
+      <c r="B15" s="108"/>
       <c r="C15" s="3" t="s">
         <v>60</v>
       </c>
@@ -3033,9 +3034,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="101"/>
-      <c r="B16" s="105" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="102"/>
+      <c r="B16" s="106" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="29" t="s">
@@ -3045,9 +3046,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="101"/>
-      <c r="B17" s="106"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="102"/>
+      <c r="B17" s="107"/>
       <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
@@ -3055,9 +3056,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="106"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="102"/>
+      <c r="B18" s="107"/>
       <c r="C18" s="30" t="s">
         <v>66</v>
       </c>
@@ -3065,9 +3066,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
-      <c r="B19" s="106"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="102"/>
+      <c r="B19" s="107"/>
       <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
@@ -3075,9 +3076,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
-      <c r="B20" s="106"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="102"/>
+      <c r="B20" s="107"/>
       <c r="C20" s="30" t="s">
         <v>70</v>
       </c>
@@ -3085,9 +3086,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="106"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="102"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
@@ -3095,9 +3096,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
-      <c r="B22" s="106"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="102"/>
+      <c r="B22" s="107"/>
       <c r="C22" s="30" t="s">
         <v>74</v>
       </c>
@@ -3105,9 +3106,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="101"/>
-      <c r="B23" s="106"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="102"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="2" t="s">
         <v>76</v>
       </c>
@@ -3115,9 +3116,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="101"/>
-      <c r="B24" s="107"/>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="102"/>
+      <c r="B24" s="108"/>
       <c r="C24" s="32" t="s">
         <v>78</v>
       </c>
@@ -3125,9 +3126,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="101"/>
-      <c r="B25" s="105" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="102"/>
+      <c r="B25" s="106" t="s">
         <v>80</v>
       </c>
       <c r="C25" s="25" t="s">
@@ -3137,9 +3138,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
-      <c r="B26" s="106"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="102"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="30" t="s">
         <v>82</v>
       </c>
@@ -3147,9 +3148,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="101"/>
-      <c r="B27" s="106"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="102"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="2" t="s">
         <v>84</v>
       </c>
@@ -3157,9 +3158,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="101"/>
-      <c r="B28" s="106"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="102"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="30" t="s">
         <v>86</v>
       </c>
@@ -3167,9 +3168,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="101"/>
-      <c r="B29" s="106"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="102"/>
+      <c r="B29" s="107"/>
       <c r="C29" s="2" t="s">
         <v>88</v>
       </c>
@@ -3177,9 +3178,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="101"/>
-      <c r="B30" s="106"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="102"/>
+      <c r="B30" s="107"/>
       <c r="C30" s="30" t="s">
         <v>90</v>
       </c>
@@ -3187,9 +3188,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="101"/>
-      <c r="B31" s="106"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="102"/>
+      <c r="B31" s="107"/>
       <c r="C31" s="2" t="s">
         <v>92</v>
       </c>
@@ -3197,9 +3198,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="101"/>
-      <c r="B32" s="106"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="102"/>
+      <c r="B32" s="107"/>
       <c r="C32" s="30" t="s">
         <v>94</v>
       </c>
@@ -3207,9 +3208,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="101"/>
-      <c r="B33" s="107"/>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="102"/>
+      <c r="B33" s="108"/>
       <c r="C33" s="27" t="s">
         <v>96</v>
       </c>
@@ -3217,9 +3218,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="101"/>
-      <c r="B34" s="105" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="102"/>
+      <c r="B34" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -3229,9 +3230,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="101"/>
-      <c r="B35" s="106"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="102"/>
+      <c r="B35" s="107"/>
       <c r="C35" s="2" t="s">
         <v>100</v>
       </c>
@@ -3239,9 +3240,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="101"/>
-      <c r="B36" s="106"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="102"/>
+      <c r="B36" s="107"/>
       <c r="C36" s="30" t="s">
         <v>102</v>
       </c>
@@ -3249,9 +3250,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="101"/>
-      <c r="B37" s="106"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="102"/>
+      <c r="B37" s="107"/>
       <c r="C37" s="2" t="s">
         <v>104</v>
       </c>
@@ -3259,9 +3260,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="101"/>
-      <c r="B38" s="106"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="102"/>
+      <c r="B38" s="107"/>
       <c r="C38" s="30" t="s">
         <v>106</v>
       </c>
@@ -3269,9 +3270,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="101"/>
-      <c r="B39" s="106"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="102"/>
+      <c r="B39" s="107"/>
       <c r="C39" s="2" t="s">
         <v>108</v>
       </c>
@@ -3279,9 +3280,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="101"/>
-      <c r="B40" s="106"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="102"/>
+      <c r="B40" s="107"/>
       <c r="C40" s="30" t="s">
         <v>110</v>
       </c>
@@ -3289,9 +3290,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="101"/>
-      <c r="B41" s="106"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="102"/>
+      <c r="B41" s="107"/>
       <c r="C41" s="2" t="s">
         <v>112</v>
       </c>
@@ -3299,9 +3300,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="101"/>
-      <c r="B42" s="107"/>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="102"/>
+      <c r="B42" s="108"/>
       <c r="C42" s="32" t="s">
         <v>114</v>
       </c>
@@ -3309,9 +3310,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="101"/>
-      <c r="B43" s="105" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="102"/>
+      <c r="B43" s="106" t="s">
         <v>116</v>
       </c>
       <c r="C43" s="25" t="s">
@@ -3321,9 +3322,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="101"/>
-      <c r="B44" s="106"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="102"/>
+      <c r="B44" s="107"/>
       <c r="C44" s="30" t="s">
         <v>118</v>
       </c>
@@ -3331,9 +3332,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="101"/>
-      <c r="B45" s="106"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="102"/>
+      <c r="B45" s="107"/>
       <c r="C45" s="2" t="s">
         <v>120</v>
       </c>
@@ -3341,9 +3342,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="101"/>
-      <c r="B46" s="106"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="102"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="30" t="s">
         <v>122</v>
       </c>
@@ -3351,9 +3352,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="101"/>
-      <c r="B47" s="106"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="102"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="2" t="s">
         <v>124</v>
       </c>
@@ -3361,9 +3362,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="101"/>
-      <c r="B48" s="106"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="102"/>
+      <c r="B48" s="107"/>
       <c r="C48" s="30" t="s">
         <v>126</v>
       </c>
@@ -3371,9 +3372,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="101"/>
-      <c r="B49" s="106"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="102"/>
+      <c r="B49" s="107"/>
       <c r="C49" s="2" t="s">
         <v>128</v>
       </c>
@@ -3381,9 +3382,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="101"/>
-      <c r="B50" s="106"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="102"/>
+      <c r="B50" s="107"/>
       <c r="C50" s="30" t="s">
         <v>130</v>
       </c>
@@ -3391,9 +3392,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="101"/>
-      <c r="B51" s="107"/>
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="102"/>
+      <c r="B51" s="108"/>
       <c r="C51" s="3" t="s">
         <v>132</v>
       </c>
@@ -3401,9 +3402,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="101"/>
-      <c r="B52" s="105" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="102"/>
+      <c r="B52" s="106" t="s">
         <v>134</v>
       </c>
       <c r="C52" s="29" t="s">
@@ -3413,9 +3414,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="101"/>
-      <c r="B53" s="106"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="102"/>
+      <c r="B53" s="107"/>
       <c r="C53" s="2" t="s">
         <v>142</v>
       </c>
@@ -3423,9 +3424,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="101"/>
-      <c r="B54" s="106"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="102"/>
+      <c r="B54" s="107"/>
       <c r="C54" s="30" t="s">
         <v>143</v>
       </c>
@@ -3433,9 +3434,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="101"/>
-      <c r="B55" s="106"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="102"/>
+      <c r="B55" s="107"/>
       <c r="C55" s="2" t="s">
         <v>144</v>
       </c>
@@ -3443,9 +3444,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="101"/>
-      <c r="B56" s="106"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="102"/>
+      <c r="B56" s="107"/>
       <c r="C56" s="30" t="s">
         <v>145</v>
       </c>
@@ -3453,9 +3454,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="101"/>
-      <c r="B57" s="106"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="102"/>
+      <c r="B57" s="107"/>
       <c r="C57" s="2" t="s">
         <v>146</v>
       </c>
@@ -3463,9 +3464,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="101"/>
-      <c r="B58" s="106"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="102"/>
+      <c r="B58" s="107"/>
       <c r="C58" s="30" t="s">
         <v>147</v>
       </c>
@@ -3473,9 +3474,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="101"/>
-      <c r="B59" s="106"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="102"/>
+      <c r="B59" s="107"/>
       <c r="C59" s="2" t="s">
         <v>148</v>
       </c>
@@ -3483,9 +3484,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="102"/>
-      <c r="B60" s="107"/>
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="103"/>
+      <c r="B60" s="108"/>
       <c r="C60" s="32" t="s">
         <v>149</v>
       </c>
@@ -3517,15 +3518,15 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
@@ -3539,11 +3540,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="101" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="111" t="s">
         <v>159</v>
       </c>
       <c r="C2" s="29" t="s">
@@ -3553,9 +3554,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
-      <c r="B3" s="108"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="102"/>
+      <c r="B3" s="109"/>
       <c r="C3" s="36" t="s">
         <v>163</v>
       </c>
@@ -3563,9 +3564,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101"/>
-      <c r="B4" s="108"/>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="102"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="38" t="s">
         <v>186</v>
       </c>
@@ -3573,9 +3574,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="101"/>
-      <c r="B5" s="109"/>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="102"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="40" t="s">
         <v>187</v>
       </c>
@@ -3583,9 +3584,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="101"/>
-      <c r="B6" s="108" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="102"/>
+      <c r="B6" s="109" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="38" t="s">
@@ -3595,9 +3596,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101"/>
-      <c r="B7" s="109"/>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="102"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="43" t="s">
         <v>165</v>
       </c>
@@ -3605,9 +3606,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="110" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="102"/>
+      <c r="B8" s="111" t="s">
         <v>169</v>
       </c>
       <c r="C8" s="29" t="s">
@@ -3617,9 +3618,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="101"/>
-      <c r="B9" s="108"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="102"/>
+      <c r="B9" s="109"/>
       <c r="C9" s="42" t="s">
         <v>171</v>
       </c>
@@ -3627,9 +3628,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="101"/>
-      <c r="B10" s="108"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="102"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="38" t="s">
         <v>172</v>
       </c>
@@ -3637,9 +3638,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="101"/>
-      <c r="B11" s="108"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="102"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="42" t="s">
         <v>173</v>
       </c>
@@ -3647,9 +3648,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="101"/>
-      <c r="B12" s="108"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="102"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="38" t="s">
         <v>177</v>
       </c>
@@ -3657,9 +3658,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="101"/>
-      <c r="B13" s="108"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="102"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="42" t="s">
         <v>178</v>
       </c>
@@ -3667,9 +3668,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="101"/>
-      <c r="B14" s="108"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="102"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="38" t="s">
         <v>179</v>
       </c>
@@ -3677,9 +3678,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="101"/>
-      <c r="B15" s="108"/>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="102"/>
+      <c r="B15" s="109"/>
       <c r="C15" s="45" t="s">
         <v>180</v>
       </c>
@@ -3687,9 +3688,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="101"/>
-      <c r="B16" s="105" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="102"/>
+      <c r="B16" s="106" t="s">
         <v>218</v>
       </c>
       <c r="C16" s="29" t="s">
@@ -3699,9 +3700,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="101"/>
-      <c r="B17" s="106"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="102"/>
+      <c r="B17" s="107"/>
       <c r="C17" s="2" t="s">
         <v>189</v>
       </c>
@@ -3709,9 +3710,9 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="106"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="102"/>
+      <c r="B18" s="107"/>
       <c r="C18" s="38" t="s">
         <v>191</v>
       </c>
@@ -3719,9 +3720,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
-      <c r="B19" s="106"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="102"/>
+      <c r="B19" s="107"/>
       <c r="C19" s="2" t="s">
         <v>192</v>
       </c>
@@ -3729,9 +3730,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
-      <c r="B20" s="106"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="102"/>
+      <c r="B20" s="107"/>
       <c r="C20" s="38" t="s">
         <v>193</v>
       </c>
@@ -3739,9 +3740,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="106"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="102"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="2" t="s">
         <v>194</v>
       </c>
@@ -3749,9 +3750,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
-      <c r="B22" s="106"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="102"/>
+      <c r="B22" s="107"/>
       <c r="C22" s="38" t="s">
         <v>200</v>
       </c>
@@ -3759,9 +3760,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="101"/>
-      <c r="B23" s="106"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="102"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="2" t="s">
         <v>201</v>
       </c>
@@ -3769,9 +3770,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="101"/>
-      <c r="B24" s="106"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="102"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="38" t="s">
         <v>210</v>
       </c>
@@ -3779,9 +3780,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="101"/>
-      <c r="B25" s="106"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="102"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="2" t="s">
         <v>211</v>
       </c>
@@ -3789,9 +3790,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
-      <c r="B26" s="106"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="102"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="38" t="s">
         <v>212</v>
       </c>
@@ -3799,9 +3800,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="101"/>
-      <c r="B27" s="106"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="102"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="2" t="s">
         <v>213</v>
       </c>
@@ -3809,9 +3810,9 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="101"/>
-      <c r="B28" s="106"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="102"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="38" t="s">
         <v>214</v>
       </c>
@@ -3819,9 +3820,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="102"/>
-      <c r="B29" s="107"/>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="103"/>
+      <c r="B29" s="108"/>
       <c r="C29" s="3" t="s">
         <v>215</v>
       </c>
@@ -3829,199 +3830,199 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="47"/>
       <c r="B30" s="47"/>
       <c r="C30" s="48"/>
       <c r="D30" s="49"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="47"/>
       <c r="B31" s="47"/>
       <c r="C31" s="48"/>
       <c r="D31" s="49"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="47"/>
       <c r="B32" s="47"/>
       <c r="C32" s="48"/>
       <c r="D32" s="49"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="47"/>
       <c r="B33" s="47"/>
       <c r="C33" s="48"/>
       <c r="D33" s="49"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="47"/>
       <c r="B34" s="47"/>
       <c r="C34" s="48"/>
       <c r="D34" s="50"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="47"/>
       <c r="B35" s="47"/>
       <c r="C35" s="48"/>
       <c r="D35" s="50"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="47"/>
       <c r="B36" s="47"/>
       <c r="C36" s="48"/>
       <c r="D36" s="50"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="47"/>
       <c r="B37" s="47"/>
       <c r="C37" s="48"/>
       <c r="D37" s="49"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="47"/>
       <c r="B38" s="47"/>
       <c r="C38" s="48"/>
       <c r="D38" s="49"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="47"/>
       <c r="B39" s="47"/>
       <c r="C39" s="48"/>
       <c r="D39" s="49"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="47"/>
       <c r="B40" s="47"/>
       <c r="C40" s="48"/>
       <c r="D40" s="49"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="47"/>
       <c r="B41" s="47"/>
       <c r="C41" s="48"/>
       <c r="D41" s="49"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="47"/>
       <c r="B42" s="47"/>
       <c r="C42" s="48"/>
       <c r="D42" s="49"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="47"/>
       <c r="B43" s="47"/>
       <c r="C43" s="48"/>
       <c r="D43" s="50"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="47"/>
       <c r="B44" s="47"/>
       <c r="C44" s="48"/>
       <c r="D44" s="50"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="47"/>
       <c r="B45" s="47"/>
       <c r="C45" s="48"/>
       <c r="D45" s="50"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="47"/>
       <c r="B46" s="47"/>
       <c r="C46" s="48"/>
       <c r="D46" s="49"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="47"/>
       <c r="B47" s="47"/>
       <c r="C47" s="48"/>
       <c r="D47" s="49"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="47"/>
       <c r="B48" s="47"/>
       <c r="C48" s="48"/>
       <c r="D48" s="49"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="47"/>
       <c r="B49" s="47"/>
       <c r="C49" s="48"/>
       <c r="D49" s="49"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="47"/>
       <c r="B50" s="47"/>
       <c r="C50" s="48"/>
       <c r="D50" s="49"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="47"/>
       <c r="B51" s="47"/>
       <c r="C51" s="48"/>
       <c r="D51" s="49"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="47"/>
       <c r="B52" s="47"/>
       <c r="C52" s="48"/>
       <c r="D52" s="50"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="47"/>
       <c r="B53" s="47"/>
       <c r="C53" s="48"/>
       <c r="D53" s="50"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="47"/>
       <c r="B54" s="47"/>
       <c r="C54" s="48"/>
       <c r="D54" s="50"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="47"/>
       <c r="B55" s="47"/>
       <c r="C55" s="48"/>
       <c r="D55" s="49"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="47"/>
       <c r="B56" s="47"/>
       <c r="C56" s="48"/>
       <c r="D56" s="49"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="47"/>
       <c r="B57" s="47"/>
       <c r="C57" s="48"/>
       <c r="D57" s="49"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="47"/>
       <c r="B58" s="47"/>
       <c r="C58" s="48"/>
       <c r="D58" s="49"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="47"/>
       <c r="B59" s="47"/>
       <c r="C59" s="48"/>
       <c r="D59" s="49"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="47"/>
       <c r="B60" s="47"/>
       <c r="C60" s="48"/>
       <c r="D60" s="49"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="49"/>
       <c r="B61" s="49"/>
       <c r="C61" s="49"/>
       <c r="D61" s="49"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="49"/>
       <c r="B62" s="49"/>
       <c r="C62" s="49"/>
@@ -4044,20 +4045,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="105.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="105.1796875" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="111" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="93" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="73" t="s">
@@ -4070,8 +4071,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="97" t="s">
         <v>260</v>
       </c>
       <c r="B2" s="81" t="s">
@@ -4084,8 +4085,8 @@
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94"/>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="95"/>
       <c r="B3" s="81" t="s">
         <v>264</v>
       </c>
@@ -4096,9 +4097,9 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="98" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="95"/>
+      <c r="B4" s="99" t="s">
         <v>267</v>
       </c>
       <c r="C4" s="86" t="s">
@@ -4108,9 +4109,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="99"/>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="95"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="88" t="s">
         <v>270</v>
       </c>
@@ -4118,8 +4119,8 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="95"/>
       <c r="B6" s="81" t="s">
         <v>271</v>
       </c>
@@ -4130,8 +4131,8 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="95"/>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="96"/>
       <c r="B7" s="81" t="s">
         <v>258</v>
       </c>
@@ -4152,6 +4153,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4160,7 +4167,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11c68bd7e868490b50c80001f2cf6c52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" xmlns:ns3="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7feae6b8f12256f9c4998c90aa2e28a" ns2:_="" ns3:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -4339,13 +4346,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4353,7 +4363,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4370,13 +4380,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>